<commit_message>
added DESeq2 diff in pipeline
</commit_message>
<xml_diff>
--- a/Docs/preconfigfile.xlsx
+++ b/Docs/preconfigfile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="2800" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="6060" yWindow="22680" windowWidth="22560" windowHeight="13920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>rawFastqDir</t>
   </si>
@@ -57,12 +57,6 @@
     <t>fastQCthreads</t>
   </si>
   <si>
-    <t>/Users/ruben/Dropbox/Projects/TestProject/Data/</t>
-  </si>
-  <si>
-    <t>/Users/ruben/Dropbox/Projects/TestProject/Results/</t>
-  </si>
-  <si>
     <t>tophat2</t>
   </si>
   <si>
@@ -175,6 +169,39 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>DESeq2</t>
+  </si>
+  <si>
+    <t>countTableOrigin</t>
+  </si>
+  <si>
+    <t>CtrlTag</t>
+  </si>
+  <si>
+    <t>TreatmentTag</t>
+  </si>
+  <si>
+    <t>Ctrl</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input count table for DESeq2 : featureCounts or HTSeq </t>
+  </si>
+  <si>
+    <t>unique tag in name of control samples</t>
+  </si>
+  <si>
+    <t>unique tag in name of treatment samples</t>
+  </si>
+  <si>
+    <t>/Users/ruben/Dropbox/Projects/RNAseqPipeline/Data/</t>
+  </si>
+  <si>
+    <t>/Users/ruben/Dropbox/Projects/RNAseqPipeline/Results/</t>
   </si>
 </sst>
 </file>
@@ -572,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -593,7 +620,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -601,10 +628,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -612,10 +639,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -626,7 +653,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -637,7 +664,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -648,7 +675,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -656,7 +683,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -667,89 +694,89 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -757,70 +784,108 @@
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added first version of DESeq2 analysis in pipeline
</commit_message>
<xml_diff>
--- a/Docs/preconfigfile.xlsx
+++ b/Docs/preconfigfile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="22680" windowWidth="22560" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="4740" yWindow="1040" windowWidth="22560" windowHeight="13920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>rawFastqDir</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>/Users/ruben/Dropbox/Projects/RNAseqPipeline/Results/</t>
+  </si>
+  <si>
+    <t>HTSeq</t>
   </si>
 </sst>
 </file>
@@ -258,8 +261,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -267,9 +272,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -661,7 +668,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -860,7 +867,7 @@
         <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
         <v>56</v>

</xml_diff>